<commit_message>
full name of student from models
</commit_message>
<xml_diff>
--- a/Attendance/sample.xlsx
+++ b/Attendance/sample.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -770,6 +770,42 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Muskan</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2021-01-15 06:23:48.161855</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2021-01-15 07:07:40.004835</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2021-01-15 07:08:33.727992</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing what i broke like an idiot
</commit_message>
<xml_diff>
--- a/Attendance/sample.xlsx
+++ b/Attendance/sample.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -806,6 +806,90 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2021-01-15 07:08:54.649707</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2021-01-15 10:19:42.224172</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2021-01-15 10:20:36.332329</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2021-01-15 10:21:41.973739</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2021-01-15 10:22:13.154482</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2021-01-15 10:22:56.788287</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2021-01-15 10:23:10.748782</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
setting up dashoard page
</commit_message>
<xml_diff>
--- a/Attendance/sample.xlsx
+++ b/Attendance/sample.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -890,6 +890,30 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2021-01-15 11:02:48.019338</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2021-01-16 18:40:41.957364</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>